<commit_message>
Right board done, all components ordered
</commit_message>
<xml_diff>
--- a/Documentation/BOM.xlsx
+++ b/Documentation/BOM.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bens1\Documents\Other\Projects\Keyboard\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF70D2EB-2836-4133-B96F-B06AB127123C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E6FA23B-4F01-424B-A16B-8A390FD8386E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" xr2:uid="{E9C67AD0-63EA-49B4-A681-DBDF8378753C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Overall" sheetId="1" r:id="rId1"/>
+    <sheet name="Electronics" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="61">
   <si>
     <t>Left board</t>
   </si>
@@ -93,6 +94,132 @@
   </si>
   <si>
     <t>Hot-swap sockets</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/user-center/orderDetails/?batchNum=W202405150613408&amp;type=myOrdersBatchSecendLevelRecord&amp;batchOrderStatus=3&amp;batchBookingStatus=0&amp;orderType=1,3</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/Adafruit/4960?qs=pBJMDPsKWf1Q%252BqeEoLnQjA%3D%3D</t>
+  </si>
+  <si>
+    <t>Neopixel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SK6812-E </t>
+  </si>
+  <si>
+    <t>GSB12J21C1EU</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/Amphenol-Commercial-Products/GSB12J21C1EU?qs=f9yNj16SXrKHw9f4qgHjvA%3D%3D</t>
+  </si>
+  <si>
+    <t>USB A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USB4510-03-1-A </t>
+  </si>
+  <si>
+    <t>USB C</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/GCT/USB4510-03-1-A?qs=7D1LtPJG0i3iod3O3OZ7LA%3D%3D</t>
+  </si>
+  <si>
+    <t>ESD Protection</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/STMicroelectronics/USBLC6-4SC6?qs=k9dH%2Fx4GHJCNdehb8zInZg%3D%3D</t>
+  </si>
+  <si>
+    <t>USBLC6-4SC6</t>
+  </si>
+  <si>
+    <t>EEPROM</t>
+  </si>
+  <si>
+    <t>M24256X-FCU6T/VF</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/STMicroelectronics/M24256X-FCU6T-VF?qs=Wj%2FVkw3K%252BMB8rPOzTsJFzg%3D%3D</t>
+  </si>
+  <si>
+    <t>LM1117LD-3.3_NOPB</t>
+  </si>
+  <si>
+    <t>Regulator</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/Texas-Instruments/LM1117LD-3.3-NOPB?qs=X1J7HmVL2ZGwq0CPAkvTtg%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/STMicroelectronics/STM32G0C1CEU6?qs=CiayqK2gdcIQOTKCTdXSKw%3D%3D</t>
+  </si>
+  <si>
+    <t>STM32G0C1CEU6</t>
+  </si>
+  <si>
+    <t>MCU</t>
+  </si>
+  <si>
+    <t>USB2533-1080AEN</t>
+  </si>
+  <si>
+    <t>USB Hub</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/Microchip-Technology/USB2533-1080AEN?qs=3i1%252BhB2xfwkiUdr5ZR6aAQ%3D%3D</t>
+  </si>
+  <si>
+    <t>CX2016SA24000D0HLLG3</t>
+  </si>
+  <si>
+    <t>USB Crystal</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/KYOCERA-AVX/CX2016SA24000D0HLLG3?qs=Imq1NPwxi75jFZJ74DHKZA%3D%3D</t>
+  </si>
+  <si>
+    <t>12k Resistor</t>
+  </si>
+  <si>
+    <t>CRGP0402F12K</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/TE-Connectivity-Holsworthy/CRGP0402F12K?qs=sGAEpiMZZMvdGkrng054tz1y1XEHv7sNAZ6rXsBbUi%252BAcnYn6U2WhA%3D%3D</t>
+  </si>
+  <si>
+    <t>10pF Capacitor</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/TAIYO-YUDEN/MCASU105SCG100DFNA01?qs=sGAEpiMZZMvsSlwiRhF8qrQG6leidpLjyNg9nggCuvzAnAwCK0sevA%3D%3D</t>
+  </si>
+  <si>
+    <t>MCASU105SCG100DFNA01</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/CUI-Devices/RIC11-31S15K7-TH?qs=HoCaDK9Nz5dozMKAx6eaHw%3D%3D</t>
+  </si>
+  <si>
+    <t>RIC11-31S15K7-TH</t>
+  </si>
+  <si>
+    <t>Encoder Long</t>
+  </si>
+  <si>
+    <t>RIC11-31S10K2-GSMT</t>
+  </si>
+  <si>
+    <t>Encoder Short</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>With VAT</t>
+  </si>
+  <si>
+    <t>Electronic components</t>
   </si>
 </sst>
 </file>
@@ -480,11 +607,12 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
+    <col min="1" max="1" width="19.3828125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.69140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.69140625" customWidth="1"/>
     <col min="7" max="7" width="13.15234375" bestFit="1" customWidth="1"/>
@@ -546,21 +674,28 @@
       <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="1">
+        <v>3.7040000000000002</v>
+      </c>
       <c r="C3" s="2">
         <v>5</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
       </c>
-      <c r="E3" s="1"/>
+      <c r="E3" s="1">
+        <v>29.94</v>
+      </c>
       <c r="F3" s="1">
         <f>B3*C3+E3</f>
-        <v>0</v>
+        <v>48.46</v>
       </c>
       <c r="G3" s="1">
-        <f t="shared" ref="G3:G13" si="0">(D3/C3)*F3</f>
-        <v>0</v>
+        <f t="shared" ref="G3:G8" si="0">(D3/C3)*F3</f>
+        <v>9.6920000000000002</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.4">
@@ -701,15 +836,21 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>60</v>
+      </c>
       <c r="B9" s="1"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G9" s="1"/>
+        <f>Electronics!F16</f>
+        <v>66.02879999999999</v>
+      </c>
+      <c r="G9" s="1">
+        <f>Electronics!G16</f>
+        <v>51.8232</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
@@ -758,11 +899,11 @@
     <row r="15" spans="1:8" x14ac:dyDescent="0.4">
       <c r="F15">
         <f>SUM(F2:F14)</f>
-        <v>160.67999999999992</v>
+        <v>275.16879999999992</v>
       </c>
       <c r="G15" s="1">
         <f>SUM(G2:G14)</f>
-        <v>101.74119480519475</v>
+        <v>163.25639480519476</v>
       </c>
     </row>
   </sheetData>
@@ -772,6 +913,454 @@
     <hyperlink ref="H5" r:id="rId3" xr:uid="{06031755-0E48-4B52-A135-CCD97071A2F2}"/>
     <hyperlink ref="H7" r:id="rId4" xr:uid="{073DC74B-9149-4257-B9E2-AD1232C79320}"/>
     <hyperlink ref="H6" r:id="rId5" xr:uid="{2B2732F6-4E4F-4001-B116-6F0F4886EA0F}"/>
+    <hyperlink ref="H3" r:id="rId6" xr:uid="{EED496C9-BF04-4699-B4BD-162FBEC4DB53}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34BACA1E-C310-409E-AC96-26FB0DBC0A23}">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="23.3046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.07421875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.69140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.15234375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="1">
+        <f>2.36 /10</f>
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="D2" s="2">
+        <v>60</v>
+      </c>
+      <c r="E2" s="2">
+        <v>54</v>
+      </c>
+      <c r="F2" s="1">
+        <f>C2*D2</f>
+        <v>14.16</v>
+      </c>
+      <c r="G2" s="1">
+        <f>(E2/D2)*F2</f>
+        <v>12.744</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.60799999999999998</v>
+      </c>
+      <c r="D3" s="2">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1">
+        <f t="shared" ref="F3:F8" si="0">C3*D3</f>
+        <v>1.8239999999999998</v>
+      </c>
+      <c r="G3" s="1">
+        <f>(E3/D3)*F3</f>
+        <v>1.2159999999999997</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.64</v>
+      </c>
+      <c r="D4" s="2">
+        <v>5</v>
+      </c>
+      <c r="E4" s="2">
+        <v>4</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" si="0"/>
+        <v>3.2</v>
+      </c>
+      <c r="G4" s="1">
+        <f>(E4/D4)*F4</f>
+        <v>2.5600000000000005</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.312</v>
+      </c>
+      <c r="D5" s="2">
+        <v>7</v>
+      </c>
+      <c r="E5" s="2">
+        <v>6</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="0"/>
+        <v>2.1840000000000002</v>
+      </c>
+      <c r="G5" s="1">
+        <f>(E5/D5)*F5</f>
+        <v>1.8720000000000001</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="D6" s="2">
+        <v>3</v>
+      </c>
+      <c r="E6" s="2">
+        <v>2</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="0"/>
+        <v>1.248</v>
+      </c>
+      <c r="G6" s="1">
+        <f>(E6/D6)*F6</f>
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="D7" s="2">
+        <v>3</v>
+      </c>
+      <c r="E7" s="2">
+        <v>2</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="0"/>
+        <v>3.5999999999999996</v>
+      </c>
+      <c r="G7" s="1">
+        <f>(E7/D7)*F7</f>
+        <v>2.3999999999999995</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="1">
+        <v>4.88</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2</v>
+      </c>
+      <c r="E8" s="2">
+        <v>2</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="0"/>
+        <v>9.76</v>
+      </c>
+      <c r="G8" s="1">
+        <f>(E8/D8)*F8</f>
+        <v>9.76</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="1">
+        <v>3.56</v>
+      </c>
+      <c r="D9" s="2">
+        <v>2</v>
+      </c>
+      <c r="E9" s="2">
+        <v>2</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" ref="F9:F14" si="1">C9*D9</f>
+        <v>7.12</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" ref="G9:G14" si="2">(E9/D9)*F9</f>
+        <v>7.12</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="D10" s="2">
+        <v>3</v>
+      </c>
+      <c r="E10" s="2">
+        <v>2</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="1"/>
+        <v>0.76800000000000002</v>
+      </c>
+      <c r="G10" s="1">
+        <f t="shared" si="2"/>
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D11" s="2">
+        <v>100</v>
+      </c>
+      <c r="E11" s="2">
+        <v>2</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+      <c r="G11" s="1">
+        <f t="shared" si="2"/>
+        <v>0.03</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D12" s="2">
+        <v>100</v>
+      </c>
+      <c r="E12" s="2">
+        <v>4</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+      <c r="G12" s="1">
+        <f t="shared" si="2"/>
+        <v>0.06</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="1">
+        <v>2.04</v>
+      </c>
+      <c r="D13" s="2">
+        <v>2</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="1"/>
+        <v>4.08</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="1">
+        <v>2.04</v>
+      </c>
+      <c r="D14" s="2">
+        <v>2</v>
+      </c>
+      <c r="E14" s="2">
+        <v>2</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="1"/>
+        <v>4.08</v>
+      </c>
+      <c r="G14" s="1">
+        <f t="shared" si="2"/>
+        <v>4.08</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="E15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" s="1">
+        <f>SUM(F2:F14)</f>
+        <v>55.023999999999994</v>
+      </c>
+      <c r="G15" s="1">
+        <f>SUM(G2:G14)</f>
+        <v>43.186</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="E16" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16" s="1">
+        <f>F15*1.2</f>
+        <v>66.02879999999999</v>
+      </c>
+      <c r="G16" s="1">
+        <f>G15*1.2</f>
+        <v>51.8232</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{D983CFCB-B47E-4FFC-ACE2-1D5346522D11}"/>
+    <hyperlink ref="H3" r:id="rId2" xr:uid="{F6079A7F-67C9-47BD-82CA-A535A57DAFDE}"/>
+    <hyperlink ref="H4" r:id="rId3" xr:uid="{E85B7AF9-ACDF-4930-A18D-85E75D98B05E}"/>
+    <hyperlink ref="H5" r:id="rId4" xr:uid="{F5421509-BC18-41D1-B772-01F3FB82DF26}"/>
+    <hyperlink ref="H6" r:id="rId5" xr:uid="{8B67E83E-E2B1-4922-A478-36E99251B04D}"/>
+    <hyperlink ref="H7" r:id="rId6" xr:uid="{4F0A6B94-918B-4E4C-97C3-5B044405F5FD}"/>
+    <hyperlink ref="H8" r:id="rId7" xr:uid="{7F0EB80B-1E6F-4345-837E-AC36CC814B3A}"/>
+    <hyperlink ref="H9" r:id="rId8" xr:uid="{7627F599-03CD-4025-BC65-62239B8A4BFF}"/>
+    <hyperlink ref="H10" r:id="rId9" xr:uid="{0F814943-9933-4C02-A2DF-041C47B331DB}"/>
+    <hyperlink ref="H11" r:id="rId10" xr:uid="{51C020E6-BBA0-459F-B3A3-F00FD88F3E52}"/>
+    <hyperlink ref="H12" r:id="rId11" xr:uid="{2682458A-6543-49D0-AC95-6E7D708F7F5C}"/>
+    <hyperlink ref="H13" r:id="rId12" xr:uid="{1D261AEF-5992-48AD-BFA6-FA847D75AED6}"/>
+    <hyperlink ref="H14" r:id="rId13" xr:uid="{A726830C-E6AB-4163-ADF5-F0ADC7D48D05}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
BOM and README updates
</commit_message>
<xml_diff>
--- a/Documentation/BOM.xlsx
+++ b/Documentation/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bens1\Documents\Other\Projects\Keyboard\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E6FA23B-4F01-424B-A16B-8A390FD8386E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C87C919C-C647-45B4-8C43-697B2AFECC89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" xr2:uid="{E9C67AD0-63EA-49B4-A681-DBDF8378753C}"/>
   </bookViews>
@@ -607,7 +607,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -675,7 +675,8 @@
         <v>7</v>
       </c>
       <c r="B3" s="1">
-        <v>3.7040000000000002</v>
+        <f>3.704+1.332</f>
+        <v>5.0360000000000005</v>
       </c>
       <c r="C3" s="2">
         <v>5</v>
@@ -688,11 +689,11 @@
       </c>
       <c r="F3" s="1">
         <f>B3*C3+E3</f>
-        <v>48.46</v>
+        <v>55.120000000000005</v>
       </c>
       <c r="G3" s="1">
         <f t="shared" ref="G3:G8" si="0">(D3/C3)*F3</f>
-        <v>9.6920000000000002</v>
+        <v>11.024000000000001</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>19</v>
@@ -899,11 +900,11 @@
     <row r="15" spans="1:8" x14ac:dyDescent="0.4">
       <c r="F15">
         <f>SUM(F2:F14)</f>
-        <v>275.16879999999992</v>
+        <v>281.82879999999989</v>
       </c>
       <c r="G15" s="1">
         <f>SUM(G2:G14)</f>
-        <v>163.25639480519476</v>
+        <v>164.58839480519475</v>
       </c>
     </row>
   </sheetData>
@@ -977,7 +978,7 @@
         <v>14.16</v>
       </c>
       <c r="G2" s="1">
-        <f>(E2/D2)*F2</f>
+        <f t="shared" ref="G2:G8" si="0">(E2/D2)*F2</f>
         <v>12.744</v>
       </c>
       <c r="H2" s="3" t="s">
@@ -1001,11 +1002,11 @@
         <v>2</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F8" si="0">C3*D3</f>
+        <f t="shared" ref="F3:F8" si="1">C3*D3</f>
         <v>1.8239999999999998</v>
       </c>
       <c r="G3" s="1">
-        <f>(E3/D3)*F3</f>
+        <f t="shared" si="0"/>
         <v>1.2159999999999997</v>
       </c>
       <c r="H3" s="3" t="s">
@@ -1029,11 +1030,11 @@
         <v>4</v>
       </c>
       <c r="F4" s="1">
+        <f t="shared" si="1"/>
+        <v>3.2</v>
+      </c>
+      <c r="G4" s="1">
         <f t="shared" si="0"/>
-        <v>3.2</v>
-      </c>
-      <c r="G4" s="1">
-        <f>(E4/D4)*F4</f>
         <v>2.5600000000000005</v>
       </c>
       <c r="H4" s="3" t="s">
@@ -1057,11 +1058,11 @@
         <v>6</v>
       </c>
       <c r="F5" s="1">
+        <f t="shared" si="1"/>
+        <v>2.1840000000000002</v>
+      </c>
+      <c r="G5" s="1">
         <f t="shared" si="0"/>
-        <v>2.1840000000000002</v>
-      </c>
-      <c r="G5" s="1">
-        <f>(E5/D5)*F5</f>
         <v>1.8720000000000001</v>
       </c>
       <c r="H5" s="3" t="s">
@@ -1085,11 +1086,11 @@
         <v>2</v>
       </c>
       <c r="F6" s="1">
+        <f t="shared" si="1"/>
+        <v>1.248</v>
+      </c>
+      <c r="G6" s="1">
         <f t="shared" si="0"/>
-        <v>1.248</v>
-      </c>
-      <c r="G6" s="1">
-        <f>(E6/D6)*F6</f>
         <v>0.83199999999999996</v>
       </c>
       <c r="H6" s="3" t="s">
@@ -1113,11 +1114,11 @@
         <v>2</v>
       </c>
       <c r="F7" s="1">
+        <f t="shared" si="1"/>
+        <v>3.5999999999999996</v>
+      </c>
+      <c r="G7" s="1">
         <f t="shared" si="0"/>
-        <v>3.5999999999999996</v>
-      </c>
-      <c r="G7" s="1">
-        <f>(E7/D7)*F7</f>
         <v>2.3999999999999995</v>
       </c>
       <c r="H7" s="3" t="s">
@@ -1141,11 +1142,11 @@
         <v>2</v>
       </c>
       <c r="F8" s="1">
+        <f t="shared" si="1"/>
+        <v>9.76</v>
+      </c>
+      <c r="G8" s="1">
         <f t="shared" si="0"/>
-        <v>9.76</v>
-      </c>
-      <c r="G8" s="1">
-        <f>(E8/D8)*F8</f>
         <v>9.76</v>
       </c>
       <c r="H8" s="3" t="s">
@@ -1169,11 +1170,11 @@
         <v>2</v>
       </c>
       <c r="F9" s="1">
-        <f t="shared" ref="F9:F14" si="1">C9*D9</f>
+        <f t="shared" ref="F9:F14" si="2">C9*D9</f>
         <v>7.12</v>
       </c>
       <c r="G9" s="1">
-        <f t="shared" ref="G9:G14" si="2">(E9/D9)*F9</f>
+        <f t="shared" ref="G9:G14" si="3">(E9/D9)*F9</f>
         <v>7.12</v>
       </c>
       <c r="H9" s="3" t="s">
@@ -1197,11 +1198,11 @@
         <v>2</v>
       </c>
       <c r="F10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.76800000000000002</v>
       </c>
       <c r="G10" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.51200000000000001</v>
       </c>
       <c r="H10" s="3" t="s">
@@ -1225,11 +1226,11 @@
         <v>2</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
       <c r="G11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.03</v>
       </c>
       <c r="H11" s="3" t="s">
@@ -1253,11 +1254,11 @@
         <v>4</v>
       </c>
       <c r="F12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
       <c r="G12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.06</v>
       </c>
       <c r="H12" s="3" t="s">
@@ -1281,11 +1282,11 @@
         <v>0</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.08</v>
       </c>
       <c r="G13" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H13" s="3" t="s">
@@ -1309,11 +1310,11 @@
         <v>2</v>
       </c>
       <c r="F14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.08</v>
       </c>
       <c r="G14" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.08</v>
       </c>
       <c r="H14" s="3" t="s">

</xml_diff>